<commit_message>
Logic for quality function and parsing action templates
</commit_message>
<xml_diff>
--- a/documentation/countries_resources_data.xlsx
+++ b/documentation/countries_resources_data.xlsx
@@ -1,32 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Vanderbilt University\Artificial Intelligence\assignments_homeworks\programming-project\world_trading_game\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1195FED2-3112-43C7-9F63-63661EF47118}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{066B723B-2CE2-4AED-9A74-82846970A6A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Countries" sheetId="1" r:id="rId1"/>
     <sheet name="Resources" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Fictional countries for the AI World Building And Trading Game</t>
   </si>
@@ -55,28 +66,70 @@
     <t>Traded and Manufactured resources in the virtual world</t>
   </si>
   <si>
-    <t>MetallicElements</t>
-  </si>
-  <si>
-    <t>MetallicAlloys</t>
-  </si>
-  <si>
-    <t>Electronics</t>
-  </si>
-  <si>
-    <t>Housing</t>
-  </si>
-  <si>
-    <t>Timber</t>
-  </si>
-  <si>
-    <t>Toy</t>
-  </si>
-  <si>
-    <t>Cotton</t>
-  </si>
-  <si>
-    <t>Garment</t>
+    <t>AvailableLand</t>
+  </si>
+  <si>
+    <t>Water</t>
+  </si>
+  <si>
+    <t>Population*</t>
+  </si>
+  <si>
+    <t>PopulationWaste</t>
+  </si>
+  <si>
+    <t>MetallicElements*</t>
+  </si>
+  <si>
+    <t>Timber*</t>
+  </si>
+  <si>
+    <t>Farm (Farm is obtained from AvailableLand and reduces the AvalilableLand amount)</t>
+  </si>
+  <si>
+    <t>FarmWaste</t>
+  </si>
+  <si>
+    <t>MetallicAlloys*</t>
+  </si>
+  <si>
+    <t>MetallicAlloysWaste*</t>
+  </si>
+  <si>
+    <t>Electronics*</t>
+  </si>
+  <si>
+    <t>ElectronicsWaste*</t>
+  </si>
+  <si>
+    <t>Housing*</t>
+  </si>
+  <si>
+    <t>HousingWaste*</t>
+  </si>
+  <si>
+    <t>Food (Food is enabled by the Farm resource, perhaps accompanied by Water)</t>
+  </si>
+  <si>
+    <t>FoodWaste</t>
+  </si>
+  <si>
+    <t>PotentialFossilEnergy (e.g., oil)</t>
+  </si>
+  <si>
+    <t>PotentialFossilEnergyUsable (e.g., oil that is extracted from land, can be exported)</t>
+  </si>
+  <si>
+    <t>PotentialFossilEnergyUsableWaste (e.g., waste as a result of the extraction process)</t>
+  </si>
+  <si>
+    <t>PotentialRenewableEnergy</t>
+  </si>
+  <si>
+    <t>PotentialRenewableEnergyUsable</t>
+  </si>
+  <si>
+    <t>PotentialRenewableEnergyUsableWaste</t>
   </si>
 </sst>
 </file>
@@ -407,8 +460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -469,10 +522,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05E33ED6-4F03-4F91-8B2F-9F04BBC15153}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -487,44 +540,114 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-    </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>